<commit_message>
meniu actualizat la detalii proiect
</commit_message>
<xml_diff>
--- a/baza_de_date.xlsx
+++ b/baza_de_date.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\facultate\an4_sem1_2023\licenta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\UniProject_Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5157DB-EF58-4703-A83B-2EC1AB2D39A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28A730E-8B3D-4C90-9BDC-165C168D2AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
   <si>
     <t>Student</t>
   </si>
@@ -72,9 +72,6 @@
     <t>An</t>
   </si>
   <si>
-    <t>Cont ulbs</t>
-  </si>
-  <si>
     <t>Grupa</t>
   </si>
   <si>
@@ -108,15 +105,6 @@
     <t>ISM</t>
   </si>
   <si>
-    <t>mACSe</t>
-  </si>
-  <si>
-    <t>mESe</t>
-  </si>
-  <si>
-    <t>Profesor</t>
-  </si>
-  <si>
     <t>Id_Profesor</t>
   </si>
   <si>
@@ -138,36 +126,6 @@
     <t>horia.caprita@ulbsibiu.ro</t>
   </si>
   <si>
-    <t>Proiect_licenta</t>
-  </si>
-  <si>
-    <t>Id_Proiect_Licenta</t>
-  </si>
-  <si>
-    <t>Candidat</t>
-  </si>
-  <si>
-    <t>Id_Candidat</t>
-  </si>
-  <si>
-    <t>Data asignarii</t>
-  </si>
-  <si>
-    <t>Id_Student_User</t>
-  </si>
-  <si>
-    <t>Nr_locuri</t>
-  </si>
-  <si>
-    <t>WEB App</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>data prezentarii</t>
-  </si>
-  <si>
     <t>primara</t>
   </si>
   <si>
@@ -267,13 +225,94 @@
     <t>id_cerinte</t>
   </si>
   <si>
-    <t>cerinta</t>
-  </si>
-  <si>
     <t>indeplinire</t>
   </si>
   <si>
     <t>observatii</t>
+  </si>
+  <si>
+    <t>0-student</t>
+  </si>
+  <si>
+    <t>1-prof</t>
+  </si>
+  <si>
+    <t>2-prof si coord</t>
+  </si>
+  <si>
+    <t>descriere</t>
+  </si>
+  <si>
+    <t>id_task</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>Teme_licenta</t>
+  </si>
+  <si>
+    <t>Id_tema</t>
+  </si>
+  <si>
+    <t>id_profesor_depcie</t>
+  </si>
+  <si>
+    <t>id_specializare</t>
+  </si>
+  <si>
+    <t>tema</t>
+  </si>
+  <si>
+    <t>cereri_teme</t>
+  </si>
+  <si>
+    <t>id_cereri</t>
+  </si>
+  <si>
+    <t>id_tema</t>
+  </si>
+  <si>
+    <t>acceptat</t>
+  </si>
+  <si>
+    <t>locuri</t>
+  </si>
+  <si>
+    <t>Id_locuri</t>
+  </si>
+  <si>
+    <t>locuri_disp</t>
+  </si>
+  <si>
+    <t>locuri_ocupate</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>id_nota</t>
+  </si>
+  <si>
+    <t>0-asteptare</t>
+  </si>
+  <si>
+    <t>1-refuzata</t>
+  </si>
+  <si>
+    <t>2-acceptata</t>
+  </si>
+  <si>
+    <t>Id_management</t>
+  </si>
+  <si>
+    <t>Teme_management</t>
+  </si>
+  <si>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>nume</t>
   </si>
 </sst>
 </file>
@@ -368,7 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -376,7 +415,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -384,7 +422,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -672,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,16 +725,20 @@
     <col min="7" max="7" width="24.6640625" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.33203125" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" customWidth="1"/>
+    <col min="16" max="16" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
-      <c r="I2" s="10" t="s">
-        <v>49</v>
+      <c r="I2" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -715,21 +756,21 @@
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="J5" s="7"/>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -749,14 +790,14 @@
         <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="J6" s="8"/>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -776,10 +817,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -787,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -799,10 +840,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -822,10 +863,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -845,10 +886,10 @@
         <v>4</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -858,10 +899,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -869,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -877,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -885,54 +926,48 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>5</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>61</v>
+        <v>46</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -943,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -952,10 +987,10 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -966,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -975,10 +1010,10 @@
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -989,7 +1024,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -998,7 +1033,7 @@
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1012,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1021,7 +1056,7 @@
         <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1035,7 +1070,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1044,7 +1079,7 @@
         <v>5</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1052,248 +1087,311 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
+      <c r="E31" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J46" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="F48" s="4"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="F49" s="4"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="13"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>29</v>
+        <v>75</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M54" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N54" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="P54" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>1</v>
       </c>
-      <c r="B55" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55">
-        <v>3</v>
-      </c>
-      <c r="D55">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F55" s="1"/>
+      <c r="J55" t="s">
+        <v>89</v>
+      </c>
+      <c r="L55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>2</v>
       </c>
-      <c r="B56" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
-      </c>
-      <c r="D56">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F56" s="1"/>
+      <c r="J56" t="s">
+        <v>90</v>
+      </c>
+      <c r="L56" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F57" s="1"/>
+      <c r="J57" t="s">
+        <v>91</v>
+      </c>
+      <c r="L57" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F58" s="1"/>
+      <c r="L58" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="3">
-        <v>1</v>
-      </c>
-      <c r="B63">
-        <v>3</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" s="7">
-        <v>45250</v>
-      </c>
-      <c r="E63" s="7">
-        <v>45483</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F59" s="1"/>
+      <c r="L59" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B62" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
secretara + admin added
</commit_message>
<xml_diff>
--- a/baza_de_date.xlsx
+++ b/baza_de_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\UniProject_Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28A730E-8B3D-4C90-9BDC-165C168D2AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3174638F-5B14-441D-9B9E-0C607F6A3A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,13 +306,13 @@
     <t>Id_management</t>
   </si>
   <si>
-    <t>Teme_management</t>
-  </si>
-  <si>
     <t>rol</t>
   </si>
   <si>
     <t>nume</t>
+  </si>
+  <si>
+    <t>management</t>
   </si>
 </sst>
 </file>
@@ -712,7 +712,7 @@
   <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
@@ -1372,10 +1372,10 @@
         <v>92</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>2</v>

</xml_diff>